<commit_message>
llama models FT corrected
</commit_message>
<xml_diff>
--- a/fine-tuning/base-llm/executability.xlsx
+++ b/fine-tuning/base-llm/executability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanm\OntoGenixLLMExperiments\fine-tuning\base-llm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39200AD-3F57-48B9-871E-58C8F9D5EA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9520711F-D89E-4935-A5FD-CDDDDE442AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="21">
   <si>
     <t>AirlinesCustomerSatisfaction</t>
   </si>
@@ -422,7 +422,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,6 +518,9 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -677,7 +680,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9289EBE8-59E9-4692-9747-E1DF5C29C5F7}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -763,6 +768,9 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -897,7 +905,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244A4901-DEA4-48E6-8612-7D3F41750B47}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -992,6 +1002,9 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>

</xml_diff>